<commit_message>
test data reading functionality from excelsheet added
</commit_message>
<xml_diff>
--- a/src/test_data/datasheet.xlsx
+++ b/src/test_data/datasheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\workspace\AppiumTesting\src\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>test case</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>tc1</t>
   </si>
@@ -42,13 +39,19 @@
   </si>
   <si>
     <t>Jan@2018</t>
+  </si>
+  <si>
+    <t>test case name</t>
+  </si>
+  <si>
+    <t>result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +63,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -79,7 +90,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -87,20 +98,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -384,38 +446,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -424,5 +490,6 @@
     <hyperlink ref="C2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test data added to excell sheet and read from different screen POM
</commit_message>
<xml_diff>
--- a/src/test_data/datasheet.xlsx
+++ b/src/test_data/datasheet.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sign_in" sheetId="1" r:id="rId1"/>
+    <sheet name="search_product" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>tc1</t>
   </si>
   <si>
-    <t>usename</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>karanbedi792@gmail.com</t>
   </si>
   <si>
@@ -45,6 +40,18 @@
   </si>
   <si>
     <t>result</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>one plus 5t cover</t>
+  </si>
+  <si>
+    <t>app_usename</t>
+  </si>
+  <si>
+    <t>app password</t>
   </si>
 </sst>
 </file>
@@ -90,7 +97,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -143,12 +150,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -163,6 +185,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -448,29 +473,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -478,10 +503,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -492,4 +517,33 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>